<commit_message>
add check imputation des heures
</commit_message>
<xml_diff>
--- a/bin/src/main/resources/templates/Feuille.xlsx
+++ b/bin/src/main/resources/templates/Feuille.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worspace\pilpose\pilpose-back\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2D355B-7629-4981-B7A0-49DA82541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEECB63-C047-4D1B-BBDE-BC872361C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,13 +57,13 @@
     <t>Chef d'équipe</t>
   </si>
   <si>
-    <t>Metiers</t>
-  </si>
-  <si>
     <t>Statut</t>
   </si>
   <si>
     <t>Indimnité</t>
+  </si>
+  <si>
+    <t>Montant Révisé</t>
   </si>
 </sst>
 </file>
@@ -114,12 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -404,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,8 +417,8 @@
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="36" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -446,23 +443,23 @@
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>